<commit_message>
seeder for all IRA Model
</commit_message>
<xml_diff>
--- a/backend/data/Descripcion_informacion_alcaparros.xlsx
+++ b/backend/data/Descripcion_informacion_alcaparros.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humbertozuluaga/Documents/PROYECTOS/PythonProjects/vueflaskformularios/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AD3762-9B31-1146-9525-9634614D48AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C861AEF-AC03-8F4E-BD09-B802294FB291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29240" yWindow="9560" windowWidth="17020" windowHeight="16320" firstSheet="2" activeTab="12" xr2:uid="{729A6A68-F19C-4A9C-AF2F-C918408CE2E9}"/>
+    <workbookView xWindow="14600" yWindow="7300" windowWidth="30560" windowHeight="19600" activeTab="1" xr2:uid="{729A6A68-F19C-4A9C-AF2F-C918408CE2E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Preguntas_en" sheetId="18" r:id="rId1"/>
     <sheet name="Preguntas" sheetId="1" r:id="rId2"/>
     <sheet name="Pregunta_periodo" sheetId="14" r:id="rId3"/>
-    <sheet name="Posibles_rtas_en" sheetId="19" r:id="rId4"/>
-    <sheet name="Posibles_rtas" sheetId="11" r:id="rId5"/>
-    <sheet name="Modalidades_cuestionario" sheetId="9" r:id="rId6"/>
-    <sheet name="Funcionarios" sheetId="8" r:id="rId7"/>
-    <sheet name="Conocimientos_en" sheetId="20" r:id="rId8"/>
-    <sheet name="Conocimientos" sheetId="3" r:id="rId9"/>
-    <sheet name="Pregunta_categoria" sheetId="16" r:id="rId10"/>
-    <sheet name="Categorias_preguntas" sheetId="15" r:id="rId11"/>
+    <sheet name="Posibles_rtas" sheetId="11" r:id="rId4"/>
+    <sheet name="Modalidades_cuestionario" sheetId="9" r:id="rId5"/>
+    <sheet name="Funcionarios" sheetId="8" r:id="rId6"/>
+    <sheet name="Conocimientos_en" sheetId="20" r:id="rId7"/>
+    <sheet name="Conocimientos" sheetId="3" r:id="rId8"/>
+    <sheet name="Pregunta_categoria" sheetId="16" r:id="rId9"/>
+    <sheet name="Categorias_preguntas" sheetId="15" r:id="rId10"/>
+    <sheet name="Networks" sheetId="22" r:id="rId11"/>
     <sheet name="Tareas" sheetId="4" r:id="rId12"/>
     <sheet name="Areas" sheetId="10" r:id="rId13"/>
     <sheet name="Recursos_en" sheetId="21" r:id="rId14"/>
@@ -33,7 +33,7 @@
     <sheet name="Periodos" sheetId="12" r:id="rId18"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Funcionarios!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Funcionarios!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="447">
   <si>
     <t>Modalidad</t>
   </si>
@@ -1334,6 +1334,69 @@
   </si>
   <si>
     <t>Technology</t>
+  </si>
+  <si>
+    <t>Pedagogical practice (classroom, evaluation, curricular development)</t>
+  </si>
+  <si>
+    <t>Logistics / administrative</t>
+  </si>
+  <si>
+    <t>My professional development</t>
+  </si>
+  <si>
+    <t>Human development</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>pedago</t>
+  </si>
+  <si>
+    <t>logis</t>
+  </si>
+  <si>
+    <t>profdev</t>
+  </si>
+  <si>
+    <t>humdev</t>
+  </si>
+  <si>
+    <t>Name_es</t>
+  </si>
+  <si>
+    <t>Name_en</t>
+  </si>
+  <si>
+    <t>Recurso</t>
+  </si>
+  <si>
+    <t>Actor</t>
+  </si>
+  <si>
+    <t>Resource</t>
+  </si>
+  <si>
+    <t>Educational Model</t>
+  </si>
+  <si>
+    <t>educ_model</t>
+  </si>
+  <si>
+    <t>resource</t>
+  </si>
+  <si>
+    <t>actor</t>
+  </si>
+  <si>
+    <t>Descripcion_es</t>
+  </si>
+  <si>
+    <t>Descripcion_en</t>
+  </si>
+  <si>
+    <t>multiple</t>
   </si>
 </sst>
 </file>
@@ -1834,7 +1897,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B1" sqref="B1:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2033,125 +2096,87 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{843E93A3-31DF-4EF9-AE2F-6CFB3493B9DA}">
-  <dimension ref="A1:B14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D37DBA92-3ACD-4ECC-B981-4ACA02D87D6F}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="49.6640625" customWidth="1"/>
+    <col min="3" max="3" width="85" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>410</v>
+      </c>
+      <c r="C1" t="s">
+        <v>411</v>
+      </c>
+      <c r="D1" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C2" t="s">
+        <v>426</v>
+      </c>
+      <c r="D2" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C3" t="s">
+        <v>427</v>
+      </c>
+      <c r="D3" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>337</v>
+      </c>
+      <c r="C4" t="s">
+        <v>428</v>
+      </c>
+      <c r="D4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>4</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>5</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>6</v>
-      </c>
-      <c r="B13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>6</v>
-      </c>
-      <c r="B14">
-        <v>4</v>
+      <c r="B5" t="s">
+        <v>338</v>
+      </c>
+      <c r="C5" t="s">
+        <v>429</v>
+      </c>
+      <c r="D5" t="s">
+        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -2160,53 +2185,73 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D37DBA92-3ACD-4ECC-B981-4ACA02D87D6F}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20120888-54FD-E547-AE07-ABA1BD347C8B}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>435</v>
+      </c>
+      <c r="C1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D1" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>358</v>
+      </c>
+      <c r="C2" t="s">
+        <v>440</v>
+      </c>
+      <c r="D2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>437</v>
+      </c>
+      <c r="C3" t="s">
+        <v>439</v>
+      </c>
+      <c r="D3" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>338</v>
+        <v>438</v>
+      </c>
+      <c r="C4" t="s">
+        <v>438</v>
+      </c>
+      <c r="D4" t="s">
+        <v>443</v>
       </c>
     </row>
   </sheetData>
@@ -2247,7 +2292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F27B6FCA-7230-448D-8AB3-EA49D7A9FD97}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -2528,7 +2573,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2811,199 +2856,239 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FA745A4-43A8-4BB6-B1EC-968C78316C93}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.1640625" customWidth="1"/>
     <col min="2" max="2" width="56.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
+    <col min="3" max="3" width="38" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="C1" t="s">
+        <v>445</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="97" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="97" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E3" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="D6" t="s">
         <v>1</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="D7" t="s">
         <v>1</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="D8" t="s">
         <v>4</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D9" t="s">
         <v>4</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>345</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="D10" t="s">
         <v>349</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>346</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="D11" t="s">
         <v>349</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>347</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="10" t="s">
+        <v>381</v>
+      </c>
+      <c r="D12" t="s">
         <v>349</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>348</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="10" t="s">
+        <v>382</v>
+      </c>
+      <c r="D13" t="s">
         <v>349</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>7</v>
       </c>
     </row>
@@ -3133,166 +3218,131 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A712BD4-B10D-4FB7-A694-614E49A14FBB}">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74871C91-0278-42EA-88A7-88F9AAA1702C}">
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.1640625" customWidth="1"/>
-    <col min="2" max="2" width="125.6640625" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" customWidth="1"/>
+    <col min="2" max="2" width="90.5" customWidth="1"/>
+    <col min="3" max="3" width="110.33203125" customWidth="1"/>
+    <col min="4" max="4" width="39.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>444</v>
+      </c>
+      <c r="C1" t="s">
+        <v>445</v>
+      </c>
+      <c r="D1" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>330</v>
+      </c>
+      <c r="C8" t="s">
         <v>389</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74871C91-0278-42EA-88A7-88F9AAA1702C}">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="8.1640625" customWidth="1"/>
-    <col min="2" max="2" width="125.6640625" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="D8">
         <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -3301,7 +3351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C87AC3E-B3BB-4E1D-8D55-92367A671B4B}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -3351,7 +3401,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95BFF06-8D57-49C9-8C64-072E2F5A5508}">
   <dimension ref="A1:G145"/>
   <sheetViews>
@@ -5850,12 +5900,132 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{688AD5BD-242D-4DBF-8ACA-D32E3996998F}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="36.1640625" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>392</v>
+      </c>
+      <c r="C3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>393</v>
+      </c>
+      <c r="C4" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>394</v>
+      </c>
+      <c r="C5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>395</v>
+      </c>
+      <c r="C6" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>396</v>
+      </c>
+      <c r="C7" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>356</v>
+      </c>
+      <c r="C8" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C9" t="s">
+        <v>358</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254AC4D3-D113-41C2-A9AD-5325EB4FEAED}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5881,7 +6051,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>391</v>
+        <v>350</v>
       </c>
       <c r="C2" t="s">
         <v>358</v>
@@ -5892,7 +6062,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>392</v>
+        <v>351</v>
       </c>
       <c r="C3" t="s">
         <v>358</v>
@@ -5903,7 +6073,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>393</v>
+        <v>352</v>
       </c>
       <c r="C4" t="s">
         <v>358</v>
@@ -5914,7 +6084,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>394</v>
+        <v>353</v>
       </c>
       <c r="C5" t="s">
         <v>358</v>
@@ -5925,7 +6095,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>395</v>
+        <v>354</v>
       </c>
       <c r="C6" t="s">
         <v>358</v>
@@ -5936,7 +6106,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>396</v>
+        <v>355</v>
       </c>
       <c r="C7" t="s">
         <v>358</v>
@@ -5958,7 +6128,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>397</v>
+        <v>357</v>
       </c>
       <c r="C9" t="s">
         <v>358</v>
@@ -5966,122 +6136,129 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254AC4D3-D113-41C2-A9AD-5325EB4FEAED}">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{843E93A3-31DF-4EF9-AE2F-6CFB3493B9DA}">
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="28.5" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>350</v>
-      </c>
-      <c r="C2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>351</v>
-      </c>
-      <c r="C3" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>352</v>
-      </c>
-      <c r="C4" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>353</v>
-      </c>
-      <c r="C5" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>354</v>
-      </c>
-      <c r="C6" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="B12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>355</v>
-      </c>
-      <c r="C7" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>356</v>
-      </c>
-      <c r="C8" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>357</v>
-      </c>
-      <c r="C9" t="s">
-        <v>358</v>
+      <c r="B13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds CVF Cultural seeder
build for PROD
</commit_message>
<xml_diff>
--- a/backend/data/Descripcion_informacion_alcaparros.xlsx
+++ b/backend/data/Descripcion_informacion_alcaparros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humbertozuluaga/Documents/PROYECTOS/PythonProjects/vueflaskformularios/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A0F787-F4D6-8048-A92E-D8E67FBFDA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7575525-F9A0-A144-944E-56F2AC2E5027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14600" yWindow="7300" windowWidth="30560" windowHeight="19600" firstSheet="4" activeTab="5" xr2:uid="{729A6A68-F19C-4A9C-AF2F-C918408CE2E9}"/>
+    <workbookView xWindow="14600" yWindow="7300" windowWidth="38420" windowHeight="21880" activeTab="2" xr2:uid="{729A6A68-F19C-4A9C-AF2F-C918408CE2E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Preguntas" sheetId="1" r:id="rId1"/>
@@ -1201,12 +1201,6 @@
     <t>What is your secondary source of knowledge and appropriation of this aspect?</t>
   </si>
   <si>
-    <t>[{"texto":"Never", "valor":0 },{"texto":"For trustworthiness", "valor":1 }, {"texto":"Due to authority", "valor":2},  {"texto":"For creativity", "valor":3},  {"texto":"For trustworthiness and authority", "valor":12},  {"texto":"For trustworthiness and creativity", "valor":13},  {"texto":"Due to authority and for creativity", "valor":23},  {"texto":"Por all the above reasons", "valor":123}]</t>
-  </si>
-  <si>
-    <t>[{"texto":"Nunca", "valor":0 },{"texto":"Por confiabilidad", "valor":1 }, {"texto":"Por autoridad", "valor":2},  {"texto":"Por creatividad", "valor":3},  {"texto":"Por confiabilidad y autoridad", "valor":12},  {"texto":"Por confiabilidad y creatividad", "valor":13},  {"texto":"Por autoridad y creatividad", "valor":23},  {"texto":"Por todas las razones anteriores", "valor":123}]</t>
-  </si>
-  <si>
     <t>[{"texto":"Definitely no", "valor":0 },{"texto":"Partially", "valor":1 },{"texto":"Definitely yes", "valor":2 }]</t>
   </si>
   <si>
@@ -1397,6 +1391,12 @@
   </si>
   <si>
     <t>Recursos_en</t>
+  </si>
+  <si>
+    <t>[{"texto":"Nunca", "valor":0 },{"texto":"Por confiabilidad", "valor":1 }, {"texto":"Por autoridad", "valor":2},  {"texto":"Por creatividad", "valor":3}]</t>
+  </si>
+  <si>
+    <t>[{"texto":"Never", "valor":0 },{"texto":"For trustworthiness", "valor":1 }, {"texto":"Due to authority", "valor":2},  {"texto":"For creativity", "valor":3}]</t>
   </si>
 </sst>
 </file>
@@ -1896,7 +1896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FA745A4-43A8-4BB6-B1EC-968C78316C93}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
@@ -1914,10 +1914,10 @@
         <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2184,10 +2184,10 @@
         <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2198,7 +2198,7 @@
         <v>317</v>
       </c>
       <c r="C2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2209,7 +2209,7 @@
         <v>318</v>
       </c>
       <c r="C3" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2220,7 +2220,7 @@
         <v>319</v>
       </c>
       <c r="C4" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2231,7 +2231,7 @@
         <v>320</v>
       </c>
       <c r="C5" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2242,7 +2242,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2253,7 +2253,7 @@
         <v>321</v>
       </c>
       <c r="C7" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2264,7 +2264,7 @@
         <v>322</v>
       </c>
       <c r="C8" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2275,7 +2275,7 @@
         <v>323</v>
       </c>
       <c r="C9" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2286,7 +2286,7 @@
         <v>324</v>
       </c>
       <c r="C10" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2297,7 +2297,7 @@
         <v>325</v>
       </c>
       <c r="C11" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2308,7 +2308,7 @@
         <v>326</v>
       </c>
       <c r="C12" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -2319,7 +2319,7 @@
         <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -2330,7 +2330,7 @@
         <v>327</v>
       </c>
       <c r="C14" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -2338,10 +2338,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C15" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
   </sheetData>
@@ -2368,10 +2368,10 @@
         <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D1" t="s">
         <v>11</v>
@@ -2385,7 +2385,7 @@
         <v>358</v>
       </c>
       <c r="C2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D2" t="s">
         <v>366</v>
@@ -2399,7 +2399,7 @@
         <v>359</v>
       </c>
       <c r="C3" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D3" t="s">
         <v>368</v>
@@ -2413,7 +2413,7 @@
         <v>360</v>
       </c>
       <c r="C4" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -2427,7 +2427,7 @@
         <v>361</v>
       </c>
       <c r="C5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D5" t="s">
         <v>364</v>
@@ -2441,7 +2441,7 @@
         <v>362</v>
       </c>
       <c r="C6" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D6" t="s">
         <v>367</v>
@@ -2779,8 +2779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74871C91-0278-42EA-88A7-88F9AAA1702C}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2796,13 +2796,13 @@
         <v>14</v>
       </c>
       <c r="B1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C1" t="s">
+        <v>442</v>
+      </c>
+      <c r="D1" t="s">
         <v>443</v>
-      </c>
-      <c r="C1" t="s">
-        <v>444</v>
-      </c>
-      <c r="D1" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2813,7 +2813,7 @@
         <v>328</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2824,13 +2824,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>383</v>
+        <v>446</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>382</v>
+        <v>447</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2841,7 +2841,7 @@
         <v>340</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -2855,7 +2855,7 @@
         <v>342</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -2869,7 +2869,7 @@
         <v>343</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -2883,7 +2883,7 @@
         <v>341</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -2897,7 +2897,7 @@
         <v>329</v>
       </c>
       <c r="C8" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -5402,16 +5402,16 @@
         <v>7380</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C143" s="6" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D143" s="6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F143" s="6" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
@@ -5419,13 +5419,13 @@
         <v>9439</v>
       </c>
       <c r="B144" s="7" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C144" s="7" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D144" s="7" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F144" s="7" t="s">
         <v>327</v>
@@ -5436,13 +5436,13 @@
         <v>7700</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C145" s="6" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D145" s="11" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F145" s="6" t="s">
         <v>322</v>
@@ -5462,7 +5462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254AC4D3-D113-41C2-A9AD-5325EB4FEAED}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -5478,10 +5478,10 @@
         <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D1" t="s">
         <v>10</v>
@@ -5495,7 +5495,7 @@
         <v>349</v>
       </c>
       <c r="C2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D2" t="s">
         <v>357</v>
@@ -5509,7 +5509,7 @@
         <v>350</v>
       </c>
       <c r="C3" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D3" t="s">
         <v>357</v>
@@ -5523,7 +5523,7 @@
         <v>351</v>
       </c>
       <c r="C4" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D4" t="s">
         <v>357</v>
@@ -5537,7 +5537,7 @@
         <v>352</v>
       </c>
       <c r="C5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D5" t="s">
         <v>357</v>
@@ -5551,7 +5551,7 @@
         <v>353</v>
       </c>
       <c r="C6" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D6" t="s">
         <v>357</v>
@@ -5565,7 +5565,7 @@
         <v>354</v>
       </c>
       <c r="C7" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D7" t="s">
         <v>357</v>
@@ -5593,7 +5593,7 @@
         <v>356</v>
       </c>
       <c r="C9" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D9" t="s">
         <v>357</v>
@@ -5750,13 +5750,13 @@
         <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5767,10 +5767,10 @@
         <v>334</v>
       </c>
       <c r="C2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5781,10 +5781,10 @@
         <v>335</v>
       </c>
       <c r="C3" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D3" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -5795,10 +5795,10 @@
         <v>336</v>
       </c>
       <c r="C4" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D4" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -5809,10 +5809,10 @@
         <v>337</v>
       </c>
       <c r="C5" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D5" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -5839,13 +5839,13 @@
         <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5856,10 +5856,10 @@
         <v>357</v>
       </c>
       <c r="C2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5867,13 +5867,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>434</v>
+      </c>
+      <c r="C3" t="s">
         <v>436</v>
       </c>
-      <c r="C3" t="s">
-        <v>438</v>
-      </c>
       <c r="D3" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -5881,13 +5881,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C4" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D4" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
   </sheetData>

</xml_diff>